<commit_message>
Added revised material on persistency
Revised chapter (web service taken out), and exercises using EF Core.
</commit_message>
<xml_diff>
--- a/Chap/DB/Tables/TableTemplate.xlsx
+++ b/Chap/DB/Tables/TableTemplate.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <t>Table name:</t>
   </si>
@@ -33,18 +33,12 @@
     <t>Allow Null</t>
   </si>
   <si>
-    <t>Default</t>
-  </si>
-  <si>
     <t>Column Name</t>
   </si>
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>Part of Key</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -66,12 +60,6 @@
     <t>is_married</t>
   </si>
   <si>
-    <t>nvarchar(50)</t>
-  </si>
-  <si>
-    <t>bit</t>
-  </si>
-  <si>
     <t>Person</t>
   </si>
   <si>
@@ -79,6 +67,21 @@
   </si>
   <si>
     <t>Origin:</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>Part of Primary Key</t>
+  </si>
+  <si>
+    <t>Default value</t>
+  </si>
+  <si>
+    <t>Is Foreign Key</t>
   </si>
 </sst>
 </file>
@@ -449,135 +452,154 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G12"/>
+  <dimension ref="B3:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="9" width="20.7109375" customWidth="1"/>
+    <col min="2" max="10" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>18</v>
+      <c r="E3" s="2"/>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>4</v>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="3" t="s">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" t="s">
-        <v>10</v>
+      <c r="H12" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>